<commit_message>
prev image deletion if not provided is implemented
</commit_message>
<xml_diff>
--- a/output/0401CS01.xlsx
+++ b/output/0401CS01.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,161 +456,6 @@
         <is>
           <t>CS</t>
         </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Semester No.</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H4" t="n">
-        <v>7</v>
-      </c>
-      <c r="I4" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Semester wise Credit Taken</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>49</v>
-      </c>
-      <c r="C5" t="n">
-        <v>44</v>
-      </c>
-      <c r="D5" t="n">
-        <v>43</v>
-      </c>
-      <c r="E5" t="n">
-        <v>47</v>
-      </c>
-      <c r="F5" t="n">
-        <v>42</v>
-      </c>
-      <c r="G5" t="n">
-        <v>40</v>
-      </c>
-      <c r="H5" t="n">
-        <v>41</v>
-      </c>
-      <c r="I5" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>SPI</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>7.96</v>
-      </c>
-      <c r="C6" t="n">
-        <v>6.82</v>
-      </c>
-      <c r="D6" t="n">
-        <v>8</v>
-      </c>
-      <c r="E6" t="n">
-        <v>8</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7.93</v>
-      </c>
-      <c r="G6" t="n">
-        <v>7.25</v>
-      </c>
-      <c r="H6" t="n">
-        <v>8.68</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8.949999999999999</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Total Credits Taken</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>49</v>
-      </c>
-      <c r="C7" t="n">
-        <v>93</v>
-      </c>
-      <c r="D7" t="n">
-        <v>136</v>
-      </c>
-      <c r="E7" t="n">
-        <v>183</v>
-      </c>
-      <c r="F7" t="n">
-        <v>225</v>
-      </c>
-      <c r="G7" t="n">
-        <v>265</v>
-      </c>
-      <c r="H7" t="n">
-        <v>306</v>
-      </c>
-      <c r="I7" t="n">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>CPI</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7.96</v>
-      </c>
-      <c r="C8" t="n">
-        <v>7.42</v>
-      </c>
-      <c r="D8" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="E8" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="F8" t="n">
-        <v>7.75</v>
-      </c>
-      <c r="G8" t="n">
-        <v>7.67</v>
-      </c>
-      <c r="H8" t="n">
-        <v>7.81</v>
-      </c>
-      <c r="I8" t="n">
-        <v>7.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>